<commit_message>
Align manager and market admin views with filtering
- Rewrite manager view to match market admin layout exactly
- Add Dashboard and Activity Plan tabs for managers
- Add Market column to manager Activity Plan view (shows all markets)
- Add filters for Business Unit, Campaign, and Medium to both views
- Manager view is read-only (no add/edit/delete capabilities)
- Both views share same statistics graphs and YTD calculations
- Market admins filter by BU/Campaign/Medium within their market
- Managers can filter across all markets

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ARO Monthly SpendDiscount report_Sep'25.xlsx
+++ b/ARO Monthly SpendDiscount report_Sep'25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://specconsa-my.sharepoint.com/personal/hein_speccon_co_za/Documents/Software Development/Projects v2/Publicis/Country Budget Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{E791B490-D9D7-4771-869B-E20E640175FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F4E7545-A8B9-4792-B2BC-7BF438B2AB34}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{E791B490-D9D7-4771-869B-E20E640175FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041D565E-ABAF-49D6-9A51-60321E940E04}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{B4B3A51A-76E0-4545-98E9-A298B3FE926E}"/>
   </bookViews>
@@ -2578,16 +2578,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -16271,7 +16262,7 @@
     <dataField name="Sum of Total Spend" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -16410,7 +16401,7 @@
     <dataField name="Sum of Total Spend" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="9">
+    <format dxfId="6">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -51738,22 +51729,22 @@
     <mergeCell ref="BQ6:BW6"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:I2 J1:J5 BO1:BO5 BX1:BX5 CG1:CG5 K1:BN20 BP1:BW47 BY1:CF47 CH1:XFD77 A3 C3:I3 A4:I5 A6 A7:I7 J7:J23 BO7:BO77 BX7:BX77 CG7:CG77 A8:B8 C8:F14 G8:I18 B9:B14 B15:F18 B19:I20 A21:I21 K21:BL23 BM21:BN31 B22:I23 B24:BL27 J28:BL31 B28:I33 J32:BN33 A34:I34 J34:BL36 BM34:BN47 B35:I36 I37:AJ43 AK37:BL44 B37:H45 J44:AJ44 I44:I45 J45:BL47 B46:I49 BP48 BY48 CD48 CF48 J48:BN52 BP49:BW77 BY49:CF77 A50:G50 I50:I52 H50:H61 B51:G60 I53:BN56 I57:I60 K57:BN62 J57:J65 B61:I62 A63:G63 I63:I65 K63:AA65 AI63:BN65 H63:H74 B64:G74 I66:BK69 BL66:BN70 T70:Z70 AI70:BK70 I70:I74 K70:S74 AA70:AA74 J70:J77 T71:U71 X71:Z71 AI71:BN71 AI72:BL72 BN72 T72:Z74 AI73:BN74 AB74:AH74 B75:I75 K75:BN77 A76:G76 H76:I77 B77:G77 B78:AA78 AI78:XFD78 I79:BK82 BL79:BM83 BN79:BN85 B79:H87 BO79:XFD90 J83:BK83 I83:I87 J84:BM84 J85:BL85 J86:BN90 B88:I88 A89:I89 B90:I90 B91:AA91 AI91:XFD91 B92:BM96 BN92:BN97 BO92:XFD104 J97:BM97 B97:I102 J98:BN98 J99:BL99 BN99 J100:BN104 A103:I103 B104:I104 B105:AA105 AI105:XFD105 B106:BN109 BO106:XFD117 B110:I115 J110:BN117 A116:G116 H116:I117 B117:G117 B118:AA118 AI118:CC118 CD118:XFD123 BO119:CC123 B119:BN129 BO124:XFD1048576 A130:BN1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ48:BW48">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BZ48:CC48">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE48">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52930,11 +52921,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5389D9F9-F732-4ABD-A2A2-5784FC0C9F5D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A3:S353"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B315" sqref="B8:B315"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G278" sqref="G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13"/>
@@ -53066,7 +53056,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="8" spans="1:19" s="48" customFormat="1">
       <c r="A8" s="276">
         <v>1.32</v>
       </c>
@@ -53109,7 +53099,7 @@
       <c r="R8" s="281"/>
       <c r="S8" s="281"/>
     </row>
-    <row r="9" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="9" spans="1:19" s="48" customFormat="1">
       <c r="A9" s="42">
         <v>1.32</v>
       </c>
@@ -53150,7 +53140,7 @@
       <c r="R9" s="50"/>
       <c r="S9" s="50"/>
     </row>
-    <row r="10" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="10" spans="1:19" s="48" customFormat="1">
       <c r="A10" s="42">
         <v>1.32</v>
       </c>
@@ -53193,7 +53183,7 @@
       <c r="R10" s="50"/>
       <c r="S10" s="50"/>
     </row>
-    <row r="11" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="11" spans="1:19" s="48" customFormat="1">
       <c r="A11" s="42">
         <v>1.32</v>
       </c>
@@ -53236,7 +53226,7 @@
       <c r="R11" s="50"/>
       <c r="S11" s="50"/>
     </row>
-    <row r="12" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="12" spans="1:19" s="48" customFormat="1">
       <c r="A12" s="42">
         <v>1.32</v>
       </c>
@@ -53279,7 +53269,7 @@
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
     </row>
-    <row r="13" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="13" spans="1:19" s="48" customFormat="1">
       <c r="A13" s="42">
         <v>1.32</v>
       </c>
@@ -53322,7 +53312,7 @@
       <c r="R13" s="50"/>
       <c r="S13" s="50"/>
     </row>
-    <row r="14" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="14" spans="1:19" s="48" customFormat="1">
       <c r="A14" s="42">
         <v>1.32</v>
       </c>
@@ -53363,7 +53353,7 @@
       <c r="R14" s="50"/>
       <c r="S14" s="50"/>
     </row>
-    <row r="15" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="15" spans="1:19" s="48" customFormat="1">
       <c r="A15" s="42">
         <v>1.32</v>
       </c>
@@ -53406,7 +53396,7 @@
       <c r="R15" s="50"/>
       <c r="S15" s="50"/>
     </row>
-    <row r="16" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="16" spans="1:19" s="48" customFormat="1">
       <c r="A16" s="42">
         <v>1.32</v>
       </c>
@@ -53451,7 +53441,7 @@
       <c r="R16" s="50"/>
       <c r="S16" s="50"/>
     </row>
-    <row r="17" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="17" spans="1:19" s="48" customFormat="1">
       <c r="A17" s="42">
         <v>1.32</v>
       </c>
@@ -53494,7 +53484,7 @@
       <c r="R17" s="50"/>
       <c r="S17" s="50"/>
     </row>
-    <row r="18" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="18" spans="1:19" s="48" customFormat="1">
       <c r="A18" s="42">
         <v>1.32</v>
       </c>
@@ -53535,7 +53525,7 @@
       <c r="R18" s="50"/>
       <c r="S18" s="50"/>
     </row>
-    <row r="19" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="19" spans="1:19" s="48" customFormat="1">
       <c r="A19" s="42">
         <v>1.32</v>
       </c>
@@ -53574,7 +53564,7 @@
       <c r="R19" s="50"/>
       <c r="S19" s="50"/>
     </row>
-    <row r="20" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="20" spans="1:19" s="48" customFormat="1">
       <c r="A20" s="42">
         <v>1.32</v>
       </c>
@@ -53613,7 +53603,7 @@
       <c r="R20" s="50"/>
       <c r="S20" s="50"/>
     </row>
-    <row r="21" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="21" spans="1:19" s="48" customFormat="1">
       <c r="A21" s="42">
         <v>1.32</v>
       </c>
@@ -53652,7 +53642,7 @@
       <c r="R21" s="50"/>
       <c r="S21" s="50"/>
     </row>
-    <row r="22" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="22" spans="1:19" s="48" customFormat="1">
       <c r="A22" s="42">
         <v>1.32</v>
       </c>
@@ -53691,7 +53681,7 @@
       <c r="R22" s="50"/>
       <c r="S22" s="50"/>
     </row>
-    <row r="23" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="23" spans="1:19" s="48" customFormat="1">
       <c r="A23" s="42">
         <v>1.32</v>
       </c>
@@ -53730,7 +53720,7 @@
       <c r="R23" s="50"/>
       <c r="S23" s="50"/>
     </row>
-    <row r="24" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="24" spans="1:19" s="48" customFormat="1">
       <c r="A24" s="42">
         <v>1.32</v>
       </c>
@@ -53769,7 +53759,7 @@
       <c r="R24" s="50"/>
       <c r="S24" s="50"/>
     </row>
-    <row r="25" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="25" spans="1:19" s="48" customFormat="1">
       <c r="A25" s="42">
         <v>1.32</v>
       </c>
@@ -53812,7 +53802,7 @@
       <c r="R25" s="50"/>
       <c r="S25" s="50"/>
     </row>
-    <row r="26" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="26" spans="1:19" s="48" customFormat="1">
       <c r="A26" s="42">
         <v>1.32</v>
       </c>
@@ -53855,7 +53845,7 @@
       <c r="R26" s="50"/>
       <c r="S26" s="50"/>
     </row>
-    <row r="27" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="27" spans="1:19" s="48" customFormat="1">
       <c r="A27" s="42">
         <v>1.32</v>
       </c>
@@ -53894,7 +53884,7 @@
       <c r="R27" s="50"/>
       <c r="S27" s="50"/>
     </row>
-    <row r="28" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="28" spans="1:19" s="48" customFormat="1">
       <c r="A28" s="42">
         <v>1.32</v>
       </c>
@@ -53933,7 +53923,7 @@
       <c r="R28" s="50"/>
       <c r="S28" s="50"/>
     </row>
-    <row r="29" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="29" spans="1:19" s="48" customFormat="1">
       <c r="A29" s="42">
         <v>1.32</v>
       </c>
@@ -53980,7 +53970,7 @@
       <c r="R29" s="50"/>
       <c r="S29" s="50"/>
     </row>
-    <row r="30" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="30" spans="1:19" s="48" customFormat="1">
       <c r="A30" s="42">
         <v>1.32</v>
       </c>
@@ -54029,7 +54019,7 @@
       <c r="R30" s="50"/>
       <c r="S30" s="50"/>
     </row>
-    <row r="31" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="31" spans="1:19" s="48" customFormat="1">
       <c r="A31" s="42">
         <v>1.32</v>
       </c>
@@ -54072,7 +54062,7 @@
       <c r="R31" s="50"/>
       <c r="S31" s="50"/>
     </row>
-    <row r="32" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="32" spans="1:19" s="48" customFormat="1">
       <c r="A32" s="42">
         <v>1.32</v>
       </c>
@@ -54117,7 +54107,7 @@
       <c r="R32" s="50"/>
       <c r="S32" s="50"/>
     </row>
-    <row r="33" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="33" spans="1:19" s="48" customFormat="1">
       <c r="A33" s="42">
         <v>1.32</v>
       </c>
@@ -54162,7 +54152,7 @@
       <c r="R33" s="50"/>
       <c r="S33" s="50"/>
     </row>
-    <row r="34" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="34" spans="1:19" s="48" customFormat="1">
       <c r="A34" s="42">
         <v>1.32</v>
       </c>
@@ -54205,7 +54195,7 @@
       <c r="R34" s="50"/>
       <c r="S34" s="50"/>
     </row>
-    <row r="35" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="35" spans="1:19" s="48" customFormat="1">
       <c r="A35" s="42">
         <v>1.32</v>
       </c>
@@ -54248,7 +54238,7 @@
       <c r="R35" s="50"/>
       <c r="S35" s="50"/>
     </row>
-    <row r="36" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="36" spans="1:19" s="48" customFormat="1">
       <c r="A36" s="42">
         <v>1.32</v>
       </c>
@@ -54289,7 +54279,7 @@
       <c r="R36" s="50"/>
       <c r="S36" s="50"/>
     </row>
-    <row r="37" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="37" spans="1:19" s="48" customFormat="1">
       <c r="A37" s="42">
         <v>1.32</v>
       </c>
@@ -54328,7 +54318,7 @@
       <c r="R37" s="50"/>
       <c r="S37" s="50"/>
     </row>
-    <row r="38" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="38" spans="1:19" s="48" customFormat="1">
       <c r="A38" s="42">
         <v>1.32</v>
       </c>
@@ -54369,7 +54359,7 @@
       <c r="R38" s="50"/>
       <c r="S38" s="50"/>
     </row>
-    <row r="39" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="39" spans="1:19" s="48" customFormat="1">
       <c r="A39" s="42">
         <v>1.32</v>
       </c>
@@ -54410,7 +54400,7 @@
       <c r="R39" s="50"/>
       <c r="S39" s="50"/>
     </row>
-    <row r="40" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="40" spans="1:19" s="48" customFormat="1">
       <c r="A40" s="42">
         <v>1.32</v>
       </c>
@@ -54451,7 +54441,7 @@
       <c r="R40" s="50"/>
       <c r="S40" s="50"/>
     </row>
-    <row r="41" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="41" spans="1:19" s="48" customFormat="1">
       <c r="A41" s="42">
         <v>1.32</v>
       </c>
@@ -54492,7 +54482,7 @@
       <c r="R41" s="50"/>
       <c r="S41" s="50"/>
     </row>
-    <row r="42" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="42" spans="1:19" s="48" customFormat="1">
       <c r="A42" s="42">
         <v>1.32</v>
       </c>
@@ -54531,7 +54521,7 @@
       <c r="R42" s="50"/>
       <c r="S42" s="50"/>
     </row>
-    <row r="43" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="43" spans="1:19" s="48" customFormat="1">
       <c r="A43" s="42">
         <v>1.32</v>
       </c>
@@ -54570,7 +54560,7 @@
       <c r="R43" s="50"/>
       <c r="S43" s="50"/>
     </row>
-    <row r="44" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="44" spans="1:19" s="48" customFormat="1">
       <c r="A44" s="42">
         <v>1.32</v>
       </c>
@@ -54609,7 +54599,7 @@
       <c r="R44" s="50"/>
       <c r="S44" s="50"/>
     </row>
-    <row r="45" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="45" spans="1:19" s="48" customFormat="1">
       <c r="A45" s="42">
         <v>1.32</v>
       </c>
@@ -54650,7 +54640,7 @@
       <c r="R45" s="50"/>
       <c r="S45" s="50"/>
     </row>
-    <row r="46" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="46" spans="1:19" s="48" customFormat="1">
       <c r="A46" s="42">
         <v>1.32</v>
       </c>
@@ -54691,7 +54681,7 @@
       <c r="R46" s="50"/>
       <c r="S46" s="50"/>
     </row>
-    <row r="47" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="47" spans="1:19" s="48" customFormat="1">
       <c r="A47" s="42">
         <v>1.32</v>
       </c>
@@ -54730,7 +54720,7 @@
       <c r="R47" s="50"/>
       <c r="S47" s="50"/>
     </row>
-    <row r="48" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="48" spans="1:19" s="48" customFormat="1">
       <c r="A48" s="42">
         <v>1.32</v>
       </c>
@@ -54769,7 +54759,7 @@
       <c r="R48" s="50"/>
       <c r="S48" s="50"/>
     </row>
-    <row r="49" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="49" spans="1:19" s="48" customFormat="1">
       <c r="A49" s="42">
         <v>1.32</v>
       </c>
@@ -54808,7 +54798,7 @@
       <c r="R49" s="50"/>
       <c r="S49" s="50"/>
     </row>
-    <row r="50" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="50" spans="1:19" s="48" customFormat="1">
       <c r="A50" s="42">
         <v>1.32</v>
       </c>
@@ -54849,7 +54839,7 @@
       <c r="R50" s="50"/>
       <c r="S50" s="50"/>
     </row>
-    <row r="51" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="51" spans="1:19" s="48" customFormat="1">
       <c r="A51" s="42">
         <v>1.32</v>
       </c>
@@ -54890,7 +54880,7 @@
       <c r="R51" s="50"/>
       <c r="S51" s="50"/>
     </row>
-    <row r="52" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="52" spans="1:19" s="48" customFormat="1">
       <c r="A52" s="42">
         <v>1.32</v>
       </c>
@@ -54931,7 +54921,7 @@
       <c r="R52" s="50"/>
       <c r="S52" s="50"/>
     </row>
-    <row r="53" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="53" spans="1:19" s="48" customFormat="1">
       <c r="A53" s="42">
         <v>1.32</v>
       </c>
@@ -54972,7 +54962,7 @@
       <c r="R53" s="50"/>
       <c r="S53" s="50"/>
     </row>
-    <row r="54" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="54" spans="1:19" s="48" customFormat="1">
       <c r="A54" s="42">
         <v>1.32</v>
       </c>
@@ -55013,7 +55003,7 @@
       <c r="R54" s="50"/>
       <c r="S54" s="50"/>
     </row>
-    <row r="55" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="55" spans="1:19" s="48" customFormat="1">
       <c r="A55" s="42">
         <v>1.32</v>
       </c>
@@ -55052,7 +55042,7 @@
       <c r="R55" s="50"/>
       <c r="S55" s="50"/>
     </row>
-    <row r="56" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="56" spans="1:19" s="48" customFormat="1">
       <c r="A56" s="42">
         <v>1.32</v>
       </c>
@@ -55091,7 +55081,7 @@
       <c r="R56" s="50"/>
       <c r="S56" s="50"/>
     </row>
-    <row r="57" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="57" spans="1:19" s="48" customFormat="1">
       <c r="A57" s="42">
         <v>1.32</v>
       </c>
@@ -55130,7 +55120,7 @@
       <c r="R57" s="50"/>
       <c r="S57" s="50"/>
     </row>
-    <row r="58" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="58" spans="1:19" s="48" customFormat="1">
       <c r="A58" s="42">
         <v>1.32</v>
       </c>
@@ -55169,7 +55159,7 @@
       <c r="R58" s="50"/>
       <c r="S58" s="50"/>
     </row>
-    <row r="59" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="59" spans="1:19" s="48" customFormat="1">
       <c r="A59" s="42">
         <v>1.32</v>
       </c>
@@ -55208,7 +55198,7 @@
       <c r="R59" s="50"/>
       <c r="S59" s="50"/>
     </row>
-    <row r="60" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="60" spans="1:19" s="48" customFormat="1">
       <c r="A60" s="248">
         <v>1.68</v>
       </c>
@@ -55251,7 +55241,7 @@
       <c r="R60" s="54"/>
       <c r="S60" s="54"/>
     </row>
-    <row r="61" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="61" spans="1:19" s="48" customFormat="1">
       <c r="A61" s="248">
         <v>1.68</v>
       </c>
@@ -55294,7 +55284,7 @@
       <c r="R61" s="54"/>
       <c r="S61" s="54"/>
     </row>
-    <row r="62" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="62" spans="1:19" s="48" customFormat="1">
       <c r="A62" s="248">
         <v>1.68</v>
       </c>
@@ -55337,7 +55327,7 @@
       <c r="R62" s="54"/>
       <c r="S62" s="54"/>
     </row>
-    <row r="63" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="63" spans="1:19" s="48" customFormat="1">
       <c r="A63" s="248">
         <v>1.68</v>
       </c>
@@ -55378,7 +55368,7 @@
       <c r="R63" s="54"/>
       <c r="S63" s="54"/>
     </row>
-    <row r="64" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="64" spans="1:19" s="48" customFormat="1">
       <c r="A64" s="248">
         <v>1.68</v>
       </c>
@@ -55431,7 +55421,7 @@
       <c r="R64" s="54"/>
       <c r="S64" s="54"/>
     </row>
-    <row r="65" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="65" spans="1:19" s="48" customFormat="1">
       <c r="A65" s="248">
         <v>1.68</v>
       </c>
@@ -55470,7 +55460,7 @@
       <c r="R65" s="54"/>
       <c r="S65" s="54"/>
     </row>
-    <row r="66" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="66" spans="1:19" s="48" customFormat="1">
       <c r="A66" s="248">
         <v>1.68</v>
       </c>
@@ -55523,7 +55513,7 @@
       <c r="R66" s="54"/>
       <c r="S66" s="54"/>
     </row>
-    <row r="67" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="67" spans="1:19" s="48" customFormat="1">
       <c r="A67" s="248">
         <v>1.68</v>
       </c>
@@ -55576,7 +55566,7 @@
       <c r="R67" s="54"/>
       <c r="S67" s="54"/>
     </row>
-    <row r="68" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="68" spans="1:19" s="48" customFormat="1">
       <c r="A68" s="248">
         <v>1.68</v>
       </c>
@@ -55617,7 +55607,7 @@
       <c r="R68" s="54"/>
       <c r="S68" s="54"/>
     </row>
-    <row r="69" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="69" spans="1:19" s="48" customFormat="1">
       <c r="A69" s="248">
         <v>1.68</v>
       </c>
@@ -55658,7 +55648,7 @@
       <c r="R69" s="54"/>
       <c r="S69" s="54"/>
     </row>
-    <row r="70" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="70" spans="1:19" s="48" customFormat="1">
       <c r="A70" s="248">
         <v>1.68</v>
       </c>
@@ -55699,7 +55689,7 @@
       <c r="R70" s="54"/>
       <c r="S70" s="54"/>
     </row>
-    <row r="71" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="71" spans="1:19" s="48" customFormat="1">
       <c r="A71" s="248">
         <v>1.68</v>
       </c>
@@ -55740,7 +55730,7 @@
       <c r="R71" s="54"/>
       <c r="S71" s="54"/>
     </row>
-    <row r="72" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="72" spans="1:19" s="48" customFormat="1">
       <c r="A72" s="248">
         <v>1.68</v>
       </c>
@@ -55791,7 +55781,7 @@
       <c r="R72" s="54"/>
       <c r="S72" s="54"/>
     </row>
-    <row r="73" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="73" spans="1:19" s="48" customFormat="1">
       <c r="A73" s="248">
         <v>1.68</v>
       </c>
@@ -55842,7 +55832,7 @@
       <c r="R73" s="54"/>
       <c r="S73" s="54"/>
     </row>
-    <row r="74" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="74" spans="1:19" s="48" customFormat="1">
       <c r="A74" s="248">
         <v>1.68</v>
       </c>
@@ -55893,7 +55883,7 @@
       <c r="R74" s="54"/>
       <c r="S74" s="54"/>
     </row>
-    <row r="75" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="75" spans="1:19" s="48" customFormat="1">
       <c r="A75" s="248">
         <v>1.68</v>
       </c>
@@ -55940,7 +55930,7 @@
       <c r="R75" s="54"/>
       <c r="S75" s="54"/>
     </row>
-    <row r="76" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="76" spans="1:19" s="48" customFormat="1">
       <c r="A76" s="248">
         <v>1.68</v>
       </c>
@@ -55981,7 +55971,7 @@
       <c r="R76" s="54"/>
       <c r="S76" s="54"/>
     </row>
-    <row r="77" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="77" spans="1:19" s="48" customFormat="1">
       <c r="A77" s="248">
         <v>1.68</v>
       </c>
@@ -56020,7 +56010,7 @@
       <c r="R77" s="54"/>
       <c r="S77" s="54"/>
     </row>
-    <row r="78" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="78" spans="1:19" s="48" customFormat="1">
       <c r="A78" s="248">
         <v>1.68</v>
       </c>
@@ -56059,7 +56049,7 @@
       <c r="R78" s="54"/>
       <c r="S78" s="54"/>
     </row>
-    <row r="79" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="79" spans="1:19" s="48" customFormat="1">
       <c r="A79" s="248">
         <v>1.68</v>
       </c>
@@ -56098,7 +56088,7 @@
       <c r="R79" s="54"/>
       <c r="S79" s="54"/>
     </row>
-    <row r="80" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="80" spans="1:19" s="48" customFormat="1">
       <c r="A80" s="248">
         <v>1.68</v>
       </c>
@@ -56137,7 +56127,7 @@
       <c r="R80" s="54"/>
       <c r="S80" s="54"/>
     </row>
-    <row r="81" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="81" spans="1:19" s="48" customFormat="1">
       <c r="A81" s="248">
         <v>1.68</v>
       </c>
@@ -56178,7 +56168,7 @@
       <c r="R81" s="54"/>
       <c r="S81" s="54"/>
     </row>
-    <row r="82" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="82" spans="1:19" s="48" customFormat="1">
       <c r="A82" s="248">
         <v>1.68</v>
       </c>
@@ -56217,7 +56207,7 @@
       <c r="R82" s="54"/>
       <c r="S82" s="54"/>
     </row>
-    <row r="83" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="83" spans="1:19" s="48" customFormat="1">
       <c r="A83" s="248">
         <v>1.68</v>
       </c>
@@ -56256,7 +56246,7 @@
       <c r="R83" s="54"/>
       <c r="S83" s="54"/>
     </row>
-    <row r="84" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="84" spans="1:19" s="48" customFormat="1">
       <c r="A84" s="248">
         <v>1.68</v>
       </c>
@@ -56295,7 +56285,7 @@
       <c r="R84" s="54"/>
       <c r="S84" s="54"/>
     </row>
-    <row r="85" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="85" spans="1:19" s="48" customFormat="1">
       <c r="A85" s="248">
         <v>1.68</v>
       </c>
@@ -56334,7 +56324,7 @@
       <c r="R85" s="54"/>
       <c r="S85" s="54"/>
     </row>
-    <row r="86" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="86" spans="1:19" s="48" customFormat="1">
       <c r="A86" s="248">
         <v>1.68</v>
       </c>
@@ -56375,7 +56365,7 @@
       <c r="R86" s="54"/>
       <c r="S86" s="54"/>
     </row>
-    <row r="87" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="87" spans="1:19" s="48" customFormat="1">
       <c r="A87" s="248">
         <v>1.68</v>
       </c>
@@ -56414,7 +56404,7 @@
       <c r="R87" s="54"/>
       <c r="S87" s="54"/>
     </row>
-    <row r="88" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="88" spans="1:19" s="48" customFormat="1">
       <c r="A88" s="248">
         <v>1.68</v>
       </c>
@@ -56455,7 +56445,7 @@
       <c r="R88" s="54"/>
       <c r="S88" s="54"/>
     </row>
-    <row r="89" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="89" spans="1:19" s="48" customFormat="1">
       <c r="A89" s="248">
         <v>1.68</v>
       </c>
@@ -56496,7 +56486,7 @@
       <c r="R89" s="54"/>
       <c r="S89" s="54"/>
     </row>
-    <row r="90" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="90" spans="1:19" s="48" customFormat="1">
       <c r="A90" s="248">
         <v>1.68</v>
       </c>
@@ -56539,7 +56529,7 @@
       <c r="R90" s="54"/>
       <c r="S90" s="54"/>
     </row>
-    <row r="91" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="91" spans="1:19" s="48" customFormat="1">
       <c r="A91" s="248">
         <v>1.68</v>
       </c>
@@ -56580,7 +56570,7 @@
       <c r="R91" s="54"/>
       <c r="S91" s="54"/>
     </row>
-    <row r="92" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="92" spans="1:19" s="48" customFormat="1">
       <c r="A92" s="248">
         <v>1.68</v>
       </c>
@@ -56621,7 +56611,7 @@
       <c r="R92" s="54"/>
       <c r="S92" s="54"/>
     </row>
-    <row r="93" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="93" spans="1:19" s="48" customFormat="1">
       <c r="A93" s="248">
         <v>1.68</v>
       </c>
@@ -56660,7 +56650,7 @@
       <c r="R93" s="54"/>
       <c r="S93" s="54"/>
     </row>
-    <row r="94" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="94" spans="1:19" s="48" customFormat="1">
       <c r="A94" s="248">
         <v>1.68</v>
       </c>
@@ -56699,7 +56689,7 @@
       <c r="R94" s="54"/>
       <c r="S94" s="54"/>
     </row>
-    <row r="95" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="95" spans="1:19" s="48" customFormat="1">
       <c r="A95" s="248">
         <v>1.68</v>
       </c>
@@ -56738,7 +56728,7 @@
       <c r="R95" s="54"/>
       <c r="S95" s="54"/>
     </row>
-    <row r="96" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="96" spans="1:19" s="48" customFormat="1">
       <c r="A96" s="248">
         <v>1.68</v>
       </c>
@@ -56777,7 +56767,7 @@
       <c r="R96" s="54"/>
       <c r="S96" s="54"/>
     </row>
-    <row r="97" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="97" spans="1:19" s="48" customFormat="1">
       <c r="A97" s="248">
         <v>1.68</v>
       </c>
@@ -56828,7 +56818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="98" spans="1:19" s="48" customFormat="1">
       <c r="A98" s="42">
         <v>1</v>
       </c>
@@ -56867,7 +56857,7 @@
       <c r="R98" s="129"/>
       <c r="S98" s="129"/>
     </row>
-    <row r="99" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="99" spans="1:19" s="48" customFormat="1">
       <c r="A99" s="42">
         <v>1</v>
       </c>
@@ -56906,7 +56896,7 @@
       <c r="R99" s="129"/>
       <c r="S99" s="129"/>
     </row>
-    <row r="100" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="100" spans="1:19" s="48" customFormat="1">
       <c r="A100" s="42">
         <v>1</v>
       </c>
@@ -56949,7 +56939,7 @@
         <v>85280.994291321083</v>
       </c>
     </row>
-    <row r="101" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="101" spans="1:19" s="48" customFormat="1">
       <c r="A101" s="42">
         <v>1</v>
       </c>
@@ -56988,7 +56978,7 @@
       <c r="R101" s="129"/>
       <c r="S101" s="129"/>
     </row>
-    <row r="102" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="102" spans="1:19" s="48" customFormat="1">
       <c r="A102" s="42">
         <v>1</v>
       </c>
@@ -57027,7 +57017,7 @@
       <c r="R102" s="129"/>
       <c r="S102" s="129"/>
     </row>
-    <row r="103" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="103" spans="1:19" s="48" customFormat="1">
       <c r="A103" s="42">
         <v>1</v>
       </c>
@@ -57066,7 +57056,7 @@
       <c r="R103" s="129"/>
       <c r="S103" s="129"/>
     </row>
-    <row r="104" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="104" spans="1:19" s="48" customFormat="1">
       <c r="A104" s="42">
         <v>1</v>
       </c>
@@ -57105,7 +57095,7 @@
       <c r="R104" s="129"/>
       <c r="S104" s="129"/>
     </row>
-    <row r="105" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="105" spans="1:19" s="48" customFormat="1">
       <c r="A105" s="42">
         <v>1</v>
       </c>
@@ -57144,7 +57134,7 @@
       <c r="R105" s="129"/>
       <c r="S105" s="129"/>
     </row>
-    <row r="106" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="106" spans="1:19" s="48" customFormat="1">
       <c r="A106" s="42">
         <v>1</v>
       </c>
@@ -57183,7 +57173,7 @@
       <c r="R106" s="129"/>
       <c r="S106" s="129"/>
     </row>
-    <row r="107" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="107" spans="1:19" s="59" customFormat="1">
       <c r="A107" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57222,7 +57212,7 @@
       <c r="R107" s="47"/>
       <c r="S107" s="47"/>
     </row>
-    <row r="108" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="108" spans="1:19" s="59" customFormat="1">
       <c r="A108" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57271,7 +57261,7 @@
       <c r="R108" s="47"/>
       <c r="S108" s="47"/>
     </row>
-    <row r="109" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="109" spans="1:19" s="59" customFormat="1">
       <c r="A109" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57310,7 +57300,7 @@
       <c r="R109" s="47"/>
       <c r="S109" s="47"/>
     </row>
-    <row r="110" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="110" spans="1:19" s="59" customFormat="1">
       <c r="A110" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57351,7 +57341,7 @@
       <c r="R110" s="47"/>
       <c r="S110" s="47"/>
     </row>
-    <row r="111" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="111" spans="1:19" s="59" customFormat="1">
       <c r="A111" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57396,7 +57386,7 @@
       <c r="R111" s="47"/>
       <c r="S111" s="47"/>
     </row>
-    <row r="112" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="112" spans="1:19" s="59" customFormat="1">
       <c r="A112" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57435,7 +57425,7 @@
       <c r="R112" s="47"/>
       <c r="S112" s="47"/>
     </row>
-    <row r="113" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="113" spans="1:19" s="59" customFormat="1">
       <c r="A113" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57474,7 +57464,7 @@
       <c r="R113" s="47"/>
       <c r="S113" s="47"/>
     </row>
-    <row r="114" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="114" spans="1:19" s="59" customFormat="1">
       <c r="A114" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57527,7 +57517,7 @@
       <c r="R114" s="47"/>
       <c r="S114" s="47"/>
     </row>
-    <row r="115" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="115" spans="1:19" s="59" customFormat="1">
       <c r="A115" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57566,7 +57556,7 @@
       <c r="R115" s="47"/>
       <c r="S115" s="47"/>
     </row>
-    <row r="116" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="116" spans="1:19" s="59" customFormat="1">
       <c r="A116" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57605,7 +57595,7 @@
       <c r="R116" s="47"/>
       <c r="S116" s="47"/>
     </row>
-    <row r="117" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="117" spans="1:19" s="59" customFormat="1">
       <c r="A117" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57644,7 +57634,7 @@
       <c r="R117" s="47"/>
       <c r="S117" s="47"/>
     </row>
-    <row r="118" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="118" spans="1:19" s="59" customFormat="1">
       <c r="A118" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57697,7 +57687,7 @@
       <c r="R118" s="47"/>
       <c r="S118" s="47"/>
     </row>
-    <row r="119" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="119" spans="1:19" s="59" customFormat="1">
       <c r="A119" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57736,7 +57726,7 @@
       <c r="R119" s="47"/>
       <c r="S119" s="47"/>
     </row>
-    <row r="120" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="120" spans="1:19" s="59" customFormat="1">
       <c r="A120" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57775,7 +57765,7 @@
       <c r="R120" s="47"/>
       <c r="S120" s="47"/>
     </row>
-    <row r="121" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="121" spans="1:19" s="59" customFormat="1">
       <c r="A121" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57820,7 +57810,7 @@
       <c r="R121" s="47"/>
       <c r="S121" s="47"/>
     </row>
-    <row r="122" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="122" spans="1:19" s="59" customFormat="1">
       <c r="A122" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57863,7 +57853,7 @@
       <c r="R122" s="47"/>
       <c r="S122" s="47"/>
     </row>
-    <row r="123" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="123" spans="1:19" s="59" customFormat="1">
       <c r="A123" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57902,7 +57892,7 @@
       <c r="R123" s="47"/>
       <c r="S123" s="47"/>
     </row>
-    <row r="124" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="124" spans="1:19" s="59" customFormat="1">
       <c r="A124" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57941,7 +57931,7 @@
       <c r="R124" s="47"/>
       <c r="S124" s="47"/>
     </row>
-    <row r="125" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="125" spans="1:19" s="59" customFormat="1">
       <c r="A125" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -57980,7 +57970,7 @@
       <c r="R125" s="47"/>
       <c r="S125" s="47"/>
     </row>
-    <row r="126" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="126" spans="1:19" s="59" customFormat="1">
       <c r="A126" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58023,7 +58013,7 @@
       <c r="R126" s="47"/>
       <c r="S126" s="47"/>
     </row>
-    <row r="127" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="127" spans="1:19" s="59" customFormat="1">
       <c r="A127" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58066,7 +58056,7 @@
       <c r="R127" s="47"/>
       <c r="S127" s="47"/>
     </row>
-    <row r="128" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="128" spans="1:19" s="59" customFormat="1">
       <c r="A128" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58105,7 +58095,7 @@
       <c r="R128" s="47"/>
       <c r="S128" s="47"/>
     </row>
-    <row r="129" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="129" spans="1:19" s="59" customFormat="1">
       <c r="A129" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58144,7 +58134,7 @@
       <c r="R129" s="47"/>
       <c r="S129" s="47"/>
     </row>
-    <row r="130" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="130" spans="1:19" s="59" customFormat="1">
       <c r="A130" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58183,7 +58173,7 @@
       <c r="R130" s="47"/>
       <c r="S130" s="47"/>
     </row>
-    <row r="131" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="131" spans="1:19" s="59" customFormat="1">
       <c r="A131" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58226,7 +58216,7 @@
       <c r="R131" s="47"/>
       <c r="S131" s="47"/>
     </row>
-    <row r="132" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="132" spans="1:19" s="59" customFormat="1">
       <c r="A132" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58269,7 +58259,7 @@
       <c r="R132" s="47"/>
       <c r="S132" s="47"/>
     </row>
-    <row r="133" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="133" spans="1:19" s="59" customFormat="1">
       <c r="A133" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58310,7 +58300,7 @@
       <c r="R133" s="47"/>
       <c r="S133" s="47"/>
     </row>
-    <row r="134" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="134" spans="1:19" s="59" customFormat="1">
       <c r="A134" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58351,7 +58341,7 @@
       <c r="R134" s="47"/>
       <c r="S134" s="47"/>
     </row>
-    <row r="135" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="135" spans="1:19" s="59" customFormat="1">
       <c r="A135" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58394,7 +58384,7 @@
       <c r="R135" s="47"/>
       <c r="S135" s="47"/>
     </row>
-    <row r="136" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="136" spans="1:19" s="59" customFormat="1">
       <c r="A136" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58435,7 +58425,7 @@
       <c r="R136" s="47"/>
       <c r="S136" s="47"/>
     </row>
-    <row r="137" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="137" spans="1:19" s="59" customFormat="1">
       <c r="A137" s="42">
         <v>0.14000000000000001</v>
       </c>
@@ -58476,7 +58466,7 @@
       <c r="R137" s="47"/>
       <c r="S137" s="47"/>
     </row>
-    <row r="138" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="138" spans="1:19" s="59" customFormat="1">
       <c r="A138" s="42">
         <v>0.39</v>
       </c>
@@ -58531,7 +58521,7 @@
       <c r="R138" s="145"/>
       <c r="S138" s="145"/>
     </row>
-    <row r="139" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="139" spans="1:19" s="59" customFormat="1">
       <c r="A139" s="42">
         <v>0.39</v>
       </c>
@@ -58574,7 +58564,7 @@
       <c r="R139" s="145"/>
       <c r="S139" s="145"/>
     </row>
-    <row r="140" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="140" spans="1:19" s="59" customFormat="1">
       <c r="A140" s="42">
         <v>0.39</v>
       </c>
@@ -58625,7 +58615,7 @@
       <c r="R140" s="145"/>
       <c r="S140" s="145"/>
     </row>
-    <row r="141" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="141" spans="1:19" s="59" customFormat="1">
       <c r="A141" s="42">
         <v>0.39</v>
       </c>
@@ -58668,7 +58658,7 @@
       <c r="R141" s="145"/>
       <c r="S141" s="145"/>
     </row>
-    <row r="142" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="142" spans="1:19" s="59" customFormat="1">
       <c r="A142" s="42">
         <v>0.39</v>
       </c>
@@ -58707,7 +58697,7 @@
       <c r="R142" s="145"/>
       <c r="S142" s="145"/>
     </row>
-    <row r="143" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="143" spans="1:19" s="59" customFormat="1">
       <c r="A143" s="42">
         <v>0.39</v>
       </c>
@@ -58746,7 +58736,7 @@
       <c r="R143" s="145"/>
       <c r="S143" s="145"/>
     </row>
-    <row r="144" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="144" spans="1:19" s="59" customFormat="1">
       <c r="A144" s="42">
         <v>0.39</v>
       </c>
@@ -58789,7 +58779,7 @@
       <c r="R144" s="145"/>
       <c r="S144" s="145"/>
     </row>
-    <row r="145" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="145" spans="1:19" s="59" customFormat="1">
       <c r="A145" s="42">
         <v>0.39</v>
       </c>
@@ -58832,7 +58822,7 @@
       <c r="R145" s="145"/>
       <c r="S145" s="145"/>
     </row>
-    <row r="146" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="146" spans="1:19" s="59" customFormat="1">
       <c r="A146" s="42">
         <v>0.39</v>
       </c>
@@ -58879,7 +58869,7 @@
       <c r="R146" s="145"/>
       <c r="S146" s="145"/>
     </row>
-    <row r="147" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="147" spans="1:19" s="59" customFormat="1">
       <c r="A147" s="42">
         <v>0.39</v>
       </c>
@@ -58922,7 +58912,7 @@
       <c r="R147" s="145"/>
       <c r="S147" s="145"/>
     </row>
-    <row r="148" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="148" spans="1:19" s="59" customFormat="1">
       <c r="A148" s="42">
         <v>0.39</v>
       </c>
@@ -58961,7 +58951,7 @@
       <c r="R148" s="145"/>
       <c r="S148" s="145"/>
     </row>
-    <row r="149" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="149" spans="1:19" s="59" customFormat="1">
       <c r="A149" s="42">
         <v>0.39</v>
       </c>
@@ -59004,7 +58994,7 @@
       <c r="R149" s="145"/>
       <c r="S149" s="145"/>
     </row>
-    <row r="150" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="150" spans="1:19" s="59" customFormat="1">
       <c r="A150" s="42">
         <v>0.39</v>
       </c>
@@ -59043,7 +59033,7 @@
       <c r="R150" s="145"/>
       <c r="S150" s="145"/>
     </row>
-    <row r="151" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="151" spans="1:19" s="59" customFormat="1">
       <c r="A151" s="42">
         <v>0.39</v>
       </c>
@@ -59086,7 +59076,7 @@
       <c r="R151" s="145"/>
       <c r="S151" s="145"/>
     </row>
-    <row r="152" spans="1:19" s="59" customFormat="1" hidden="1">
+    <row r="152" spans="1:19" s="59" customFormat="1">
       <c r="A152" s="42">
         <v>0.39</v>
       </c>
@@ -59129,7 +59119,7 @@
       <c r="R152" s="145"/>
       <c r="S152" s="145"/>
     </row>
-    <row r="153" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="153" spans="1:19" s="48" customFormat="1">
       <c r="A153" s="42">
         <v>0.39</v>
       </c>
@@ -59168,7 +59158,7 @@
       <c r="R153" s="145"/>
       <c r="S153" s="145"/>
     </row>
-    <row r="154" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="154" spans="1:19" s="48" customFormat="1">
       <c r="A154" s="42">
         <v>0.39</v>
       </c>
@@ -59215,7 +59205,7 @@
       <c r="R154" s="145"/>
       <c r="S154" s="145"/>
     </row>
-    <row r="155" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="155" spans="1:19" s="48" customFormat="1">
       <c r="A155" s="42">
         <v>0.39</v>
       </c>
@@ -59262,7 +59252,7 @@
       <c r="R155" s="145"/>
       <c r="S155" s="145"/>
     </row>
-    <row r="156" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="156" spans="1:19" s="48" customFormat="1">
       <c r="A156" s="42">
         <v>0.39</v>
       </c>
@@ -59305,7 +59295,7 @@
       <c r="R156" s="145"/>
       <c r="S156" s="145"/>
     </row>
-    <row r="157" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="157" spans="1:19" s="48" customFormat="1">
       <c r="A157" s="42">
         <v>0.39</v>
       </c>
@@ -59348,7 +59338,7 @@
       <c r="R157" s="145"/>
       <c r="S157" s="145"/>
     </row>
-    <row r="158" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="158" spans="1:19" s="48" customFormat="1">
       <c r="A158" s="42">
         <v>0.39</v>
       </c>
@@ -59401,7 +59391,7 @@
       <c r="R158" s="145"/>
       <c r="S158" s="145"/>
     </row>
-    <row r="159" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="159" spans="1:19" s="48" customFormat="1">
       <c r="A159" s="42">
         <v>0.39</v>
       </c>
@@ -59440,7 +59430,7 @@
       <c r="R159" s="145"/>
       <c r="S159" s="145"/>
     </row>
-    <row r="160" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="160" spans="1:19" s="48" customFormat="1">
       <c r="A160" s="42">
         <v>0.39</v>
       </c>
@@ -59479,7 +59469,7 @@
       <c r="R160" s="145"/>
       <c r="S160" s="145"/>
     </row>
-    <row r="161" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="161" spans="1:19" s="48" customFormat="1">
       <c r="A161" s="42">
         <v>0.39</v>
       </c>
@@ -59518,7 +59508,7 @@
       <c r="R161" s="145"/>
       <c r="S161" s="145"/>
     </row>
-    <row r="162" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="162" spans="1:19" s="48" customFormat="1">
       <c r="A162" s="42">
         <v>0.39</v>
       </c>
@@ -59557,7 +59547,7 @@
       <c r="R162" s="145"/>
       <c r="S162" s="145"/>
     </row>
-    <row r="163" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="163" spans="1:19" s="48" customFormat="1">
       <c r="A163" s="42">
         <v>0.39</v>
       </c>
@@ -59602,7 +59592,7 @@
       <c r="R163" s="145"/>
       <c r="S163" s="145"/>
     </row>
-    <row r="164" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="164" spans="1:19" s="48" customFormat="1">
       <c r="A164" s="42">
         <v>0.39</v>
       </c>
@@ -59651,7 +59641,7 @@
       <c r="R164" s="145"/>
       <c r="S164" s="145"/>
     </row>
-    <row r="165" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="165" spans="1:19" s="48" customFormat="1">
       <c r="A165" s="42">
         <v>0.39</v>
       </c>
@@ -59698,7 +59688,7 @@
       <c r="R165" s="145"/>
       <c r="S165" s="145"/>
     </row>
-    <row r="166" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="166" spans="1:19" s="48" customFormat="1">
       <c r="A166" s="42">
         <v>0.39</v>
       </c>
@@ -59739,7 +59729,7 @@
       <c r="R166" s="145"/>
       <c r="S166" s="145"/>
     </row>
-    <row r="167" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="167" spans="1:19" s="48" customFormat="1">
       <c r="A167" s="42">
         <v>0.39</v>
       </c>
@@ -59778,7 +59768,7 @@
       <c r="R167" s="145"/>
       <c r="S167" s="145"/>
     </row>
-    <row r="168" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="168" spans="1:19" s="48" customFormat="1">
       <c r="A168" s="42">
         <v>0.39</v>
       </c>
@@ -59829,7 +59819,7 @@
       <c r="R168" s="145"/>
       <c r="S168" s="145"/>
     </row>
-    <row r="169" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="169" spans="1:19" s="48" customFormat="1">
       <c r="A169" s="42">
         <v>0.39</v>
       </c>
@@ -59868,7 +59858,7 @@
       <c r="R169" s="145"/>
       <c r="S169" s="145"/>
     </row>
-    <row r="170" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="170" spans="1:19" s="48" customFormat="1">
       <c r="A170" s="42">
         <v>0.39</v>
       </c>
@@ -59907,7 +59897,7 @@
       <c r="R170" s="145"/>
       <c r="S170" s="145"/>
     </row>
-    <row r="171" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="171" spans="1:19" s="48" customFormat="1">
       <c r="A171" s="42">
         <v>0.39</v>
       </c>
@@ -59946,7 +59936,7 @@
       <c r="R171" s="145"/>
       <c r="S171" s="145"/>
     </row>
-    <row r="172" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="172" spans="1:19" s="48" customFormat="1">
       <c r="A172" s="42">
         <v>0.39</v>
       </c>
@@ -59989,7 +59979,7 @@
       <c r="R172" s="145"/>
       <c r="S172" s="145"/>
     </row>
-    <row r="173" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="173" spans="1:19" s="48" customFormat="1">
       <c r="A173" s="42">
         <v>0.39</v>
       </c>
@@ -60032,7 +60022,7 @@
       <c r="R173" s="145"/>
       <c r="S173" s="145"/>
     </row>
-    <row r="174" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="174" spans="1:19" s="48" customFormat="1">
       <c r="A174" s="42">
         <v>0.39</v>
       </c>
@@ -60075,7 +60065,7 @@
       <c r="R174" s="145"/>
       <c r="S174" s="145"/>
     </row>
-    <row r="175" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="175" spans="1:19" s="48" customFormat="1">
       <c r="A175" s="42">
         <v>0.39</v>
       </c>
@@ -60114,7 +60104,7 @@
       <c r="R175" s="145"/>
       <c r="S175" s="145"/>
     </row>
-    <row r="176" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="176" spans="1:19" s="48" customFormat="1">
       <c r="A176" s="42">
         <v>0.39</v>
       </c>
@@ -60153,7 +60143,7 @@
       <c r="R176" s="145"/>
       <c r="S176" s="145"/>
     </row>
-    <row r="177" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="177" spans="1:19" s="48" customFormat="1">
       <c r="A177" s="42">
         <v>0.39</v>
       </c>
@@ -60194,7 +60184,7 @@
       <c r="R177" s="145"/>
       <c r="S177" s="145"/>
     </row>
-    <row r="178" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="178" spans="1:19" s="48" customFormat="1">
       <c r="A178" s="42">
         <v>0.39</v>
       </c>
@@ -60235,7 +60225,7 @@
       <c r="R178" s="145"/>
       <c r="S178" s="145"/>
     </row>
-    <row r="179" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="179" spans="1:19" s="48" customFormat="1">
       <c r="A179" s="42">
         <v>0.39</v>
       </c>
@@ -60276,7 +60266,7 @@
       <c r="R179" s="145"/>
       <c r="S179" s="145"/>
     </row>
-    <row r="180" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="180" spans="1:19" s="48" customFormat="1">
       <c r="A180" s="42">
         <v>0.39</v>
       </c>
@@ -60317,7 +60307,7 @@
       <c r="R180" s="145"/>
       <c r="S180" s="145"/>
     </row>
-    <row r="181" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="181" spans="1:19" s="48" customFormat="1">
       <c r="A181" s="42">
         <v>0.39</v>
       </c>
@@ -60356,7 +60346,7 @@
       <c r="R181" s="145"/>
       <c r="S181" s="145"/>
     </row>
-    <row r="182" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="182" spans="1:19" s="48" customFormat="1">
       <c r="A182" s="42">
         <v>0.39</v>
       </c>
@@ -60395,7 +60385,7 @@
       <c r="R182" s="145"/>
       <c r="S182" s="145"/>
     </row>
-    <row r="183" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="183" spans="1:19" s="48" customFormat="1">
       <c r="A183" s="42">
         <v>0.39</v>
       </c>
@@ -60434,7 +60424,7 @@
       <c r="R183" s="145"/>
       <c r="S183" s="145"/>
     </row>
-    <row r="184" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="184" spans="1:19" s="48" customFormat="1">
       <c r="A184" s="42">
         <v>0.39</v>
       </c>
@@ -60473,7 +60463,7 @@
       <c r="R184" s="145"/>
       <c r="S184" s="145"/>
     </row>
-    <row r="185" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="185" spans="1:19" s="48" customFormat="1">
       <c r="A185" s="42">
         <v>0.39</v>
       </c>
@@ -60512,7 +60502,7 @@
       <c r="R185" s="145"/>
       <c r="S185" s="145"/>
     </row>
-    <row r="186" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="186" spans="1:19" s="48" customFormat="1">
       <c r="A186" s="42">
         <v>0.39</v>
       </c>
@@ -60551,7 +60541,7 @@
       <c r="R186" s="145"/>
       <c r="S186" s="145"/>
     </row>
-    <row r="187" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="187" spans="1:19" s="48" customFormat="1">
       <c r="A187" s="42">
         <v>0.39</v>
       </c>
@@ -60590,7 +60580,7 @@
       <c r="R187" s="145"/>
       <c r="S187" s="145"/>
     </row>
-    <row r="188" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="188" spans="1:19" s="48" customFormat="1">
       <c r="A188" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60633,7 +60623,7 @@
       <c r="R188" s="61"/>
       <c r="S188" s="61"/>
     </row>
-    <row r="189" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="189" spans="1:19" s="48" customFormat="1">
       <c r="A189" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60674,7 +60664,7 @@
       <c r="R189" s="61"/>
       <c r="S189" s="61"/>
     </row>
-    <row r="190" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="190" spans="1:19" s="48" customFormat="1">
       <c r="A190" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60715,7 +60705,7 @@
       <c r="R190" s="61"/>
       <c r="S190" s="61"/>
     </row>
-    <row r="191" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="191" spans="1:19" s="48" customFormat="1">
       <c r="A191" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60756,7 +60746,7 @@
       <c r="R191" s="61"/>
       <c r="S191" s="61"/>
     </row>
-    <row r="192" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="192" spans="1:19" s="48" customFormat="1">
       <c r="A192" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60797,7 +60787,7 @@
       <c r="R192" s="61"/>
       <c r="S192" s="61"/>
     </row>
-    <row r="193" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="193" spans="1:19" s="48" customFormat="1">
       <c r="A193" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60840,7 +60830,7 @@
       <c r="R193" s="61"/>
       <c r="S193" s="61"/>
     </row>
-    <row r="194" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="194" spans="1:19" s="48" customFormat="1">
       <c r="A194" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60883,7 +60873,7 @@
       <c r="R194" s="61"/>
       <c r="S194" s="61"/>
     </row>
-    <row r="195" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="195" spans="1:19" s="48" customFormat="1">
       <c r="A195" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60926,7 +60916,7 @@
       <c r="R195" s="61"/>
       <c r="S195" s="61"/>
     </row>
-    <row r="196" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="196" spans="1:19" s="48" customFormat="1">
       <c r="A196" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -60963,7 +60953,7 @@
       <c r="R196" s="61"/>
       <c r="S196" s="61"/>
     </row>
-    <row r="197" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="197" spans="1:19" s="48" customFormat="1">
       <c r="A197" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61002,7 +60992,7 @@
       <c r="R197" s="61"/>
       <c r="S197" s="61"/>
     </row>
-    <row r="198" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="198" spans="1:19" s="48" customFormat="1">
       <c r="A198" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61041,7 +61031,7 @@
       <c r="R198" s="61"/>
       <c r="S198" s="61"/>
     </row>
-    <row r="199" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="199" spans="1:19" s="48" customFormat="1">
       <c r="A199" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61080,7 +61070,7 @@
       <c r="R199" s="61"/>
       <c r="S199" s="61"/>
     </row>
-    <row r="200" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="200" spans="1:19" s="48" customFormat="1">
       <c r="A200" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61119,7 +61109,7 @@
       <c r="R200" s="61"/>
       <c r="S200" s="61"/>
     </row>
-    <row r="201" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="201" spans="1:19" s="48" customFormat="1">
       <c r="A201" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61156,7 +61146,7 @@
       <c r="R201" s="61"/>
       <c r="S201" s="61"/>
     </row>
-    <row r="202" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="202" spans="1:19" s="48" customFormat="1">
       <c r="A202" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61193,7 +61183,7 @@
       <c r="R202" s="61"/>
       <c r="S202" s="61"/>
     </row>
-    <row r="203" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="203" spans="1:19" s="48" customFormat="1">
       <c r="A203" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61232,7 +61222,7 @@
       <c r="R203" s="61"/>
       <c r="S203" s="61"/>
     </row>
-    <row r="204" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="204" spans="1:19" s="48" customFormat="1">
       <c r="A204" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61271,7 +61261,7 @@
       <c r="R204" s="61"/>
       <c r="S204" s="61"/>
     </row>
-    <row r="205" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="205" spans="1:19" s="48" customFormat="1">
       <c r="A205" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -61310,7 +61300,7 @@
       <c r="R205" s="61"/>
       <c r="S205" s="61"/>
     </row>
-    <row r="206" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="206" spans="1:19" s="48" customFormat="1">
       <c r="A206" s="248">
         <v>0.76</v>
       </c>
@@ -61349,7 +61339,7 @@
       <c r="R206" s="58"/>
       <c r="S206" s="58"/>
     </row>
-    <row r="207" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="207" spans="1:19" s="48" customFormat="1">
       <c r="A207" s="248">
         <v>0.76</v>
       </c>
@@ -61394,7 +61384,7 @@
       <c r="R207" s="58"/>
       <c r="S207" s="58"/>
     </row>
-    <row r="208" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="208" spans="1:19" s="48" customFormat="1">
       <c r="A208" s="248">
         <v>0.76</v>
       </c>
@@ -61433,7 +61423,7 @@
       <c r="R208" s="58"/>
       <c r="S208" s="58"/>
     </row>
-    <row r="209" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="209" spans="1:19" s="48" customFormat="1">
       <c r="A209" s="248">
         <v>0.76</v>
       </c>
@@ -61490,7 +61480,7 @@
       <c r="R209" s="58"/>
       <c r="S209" s="58"/>
     </row>
-    <row r="210" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="210" spans="1:19" s="48" customFormat="1">
       <c r="A210" s="248">
         <v>0.76</v>
       </c>
@@ -61537,7 +61527,7 @@
       <c r="R210" s="58"/>
       <c r="S210" s="58"/>
     </row>
-    <row r="211" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="211" spans="1:19" s="48" customFormat="1">
       <c r="A211" s="248">
         <v>0.76</v>
       </c>
@@ -61576,7 +61566,7 @@
       <c r="R211" s="58"/>
       <c r="S211" s="58"/>
     </row>
-    <row r="212" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="212" spans="1:19" s="48" customFormat="1">
       <c r="A212" s="248">
         <v>0.76</v>
       </c>
@@ -61615,7 +61605,7 @@
       <c r="R212" s="58"/>
       <c r="S212" s="58"/>
     </row>
-    <row r="213" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="213" spans="1:19" s="48" customFormat="1">
       <c r="A213" s="248">
         <v>0.76</v>
       </c>
@@ -61654,7 +61644,7 @@
       <c r="R213" s="58"/>
       <c r="S213" s="58"/>
     </row>
-    <row r="214" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="214" spans="1:19" s="48" customFormat="1">
       <c r="A214" s="248">
         <v>0.76</v>
       </c>
@@ -61697,7 +61687,7 @@
       <c r="R214" s="58"/>
       <c r="S214" s="58"/>
     </row>
-    <row r="215" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="215" spans="1:19" s="48" customFormat="1">
       <c r="A215" s="248">
         <v>0.76</v>
       </c>
@@ -61742,7 +61732,7 @@
       <c r="R215" s="58"/>
       <c r="S215" s="58"/>
     </row>
-    <row r="216" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="216" spans="1:19" s="48" customFormat="1">
       <c r="A216" s="248">
         <v>0.76</v>
       </c>
@@ -61785,7 +61775,7 @@
       <c r="R216" s="58"/>
       <c r="S216" s="58"/>
     </row>
-    <row r="217" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="217" spans="1:19" s="48" customFormat="1">
       <c r="A217" s="248">
         <v>0.76</v>
       </c>
@@ -61824,7 +61814,7 @@
       <c r="R217" s="58"/>
       <c r="S217" s="58"/>
     </row>
-    <row r="218" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="218" spans="1:19" s="48" customFormat="1">
       <c r="A218" s="248">
         <v>0.76</v>
       </c>
@@ -61867,7 +61857,7 @@
       <c r="R218" s="58"/>
       <c r="S218" s="58"/>
     </row>
-    <row r="219" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="219" spans="1:19" s="48" customFormat="1">
       <c r="A219" s="248">
         <v>0.76</v>
       </c>
@@ -61910,7 +61900,7 @@
       <c r="R219" s="58"/>
       <c r="S219" s="58"/>
     </row>
-    <row r="220" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="220" spans="1:19" s="48" customFormat="1">
       <c r="A220" s="248">
         <v>0.76</v>
       </c>
@@ -61955,7 +61945,7 @@
       <c r="R220" s="58"/>
       <c r="S220" s="58"/>
     </row>
-    <row r="221" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="221" spans="1:19" s="48" customFormat="1">
       <c r="A221" s="248">
         <v>0.76</v>
       </c>
@@ -61996,7 +61986,7 @@
       <c r="R221" s="58"/>
       <c r="S221" s="58"/>
     </row>
-    <row r="222" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="222" spans="1:19" s="48" customFormat="1">
       <c r="A222" s="248">
         <v>0.76</v>
       </c>
@@ -62043,7 +62033,7 @@
       <c r="R222" s="58"/>
       <c r="S222" s="58"/>
     </row>
-    <row r="223" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="223" spans="1:19" s="48" customFormat="1">
       <c r="A223" s="248">
         <v>0.76</v>
       </c>
@@ -62082,7 +62072,7 @@
       <c r="R223" s="58"/>
       <c r="S223" s="58"/>
     </row>
-    <row r="224" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="224" spans="1:19" s="48" customFormat="1">
       <c r="A224" s="248">
         <v>0.76</v>
       </c>
@@ -62127,7 +62117,7 @@
       <c r="R224" s="58"/>
       <c r="S224" s="58"/>
     </row>
-    <row r="225" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="225" spans="1:19" s="48" customFormat="1">
       <c r="A225" s="248">
         <v>0.76</v>
       </c>
@@ -62170,7 +62160,7 @@
       <c r="R225" s="58"/>
       <c r="S225" s="58"/>
     </row>
-    <row r="226" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="226" spans="1:19" s="48" customFormat="1">
       <c r="A226" s="248">
         <v>0.76</v>
       </c>
@@ -62211,7 +62201,7 @@
       <c r="R226" s="58"/>
       <c r="S226" s="58"/>
     </row>
-    <row r="227" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="227" spans="1:19" s="48" customFormat="1">
       <c r="A227" s="248">
         <v>0.76</v>
       </c>
@@ -62252,7 +62242,7 @@
       <c r="R227" s="58"/>
       <c r="S227" s="58"/>
     </row>
-    <row r="228" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="228" spans="1:19" s="48" customFormat="1">
       <c r="A228" s="248">
         <v>0.76</v>
       </c>
@@ -62293,7 +62283,7 @@
       <c r="R228" s="58"/>
       <c r="S228" s="58"/>
     </row>
-    <row r="229" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="229" spans="1:19" s="48" customFormat="1">
       <c r="A229" s="248">
         <v>0.76</v>
       </c>
@@ -62336,7 +62326,7 @@
       <c r="R229" s="58"/>
       <c r="S229" s="58"/>
     </row>
-    <row r="230" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="230" spans="1:19" s="48" customFormat="1">
       <c r="A230" s="248">
         <v>0.76</v>
       </c>
@@ -62387,7 +62377,7 @@
       <c r="R230" s="58"/>
       <c r="S230" s="58"/>
     </row>
-    <row r="231" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="231" spans="1:19" s="48" customFormat="1">
       <c r="A231" s="248">
         <v>0.76</v>
       </c>
@@ -62428,7 +62418,7 @@
       <c r="R231" s="58"/>
       <c r="S231" s="58"/>
     </row>
-    <row r="232" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="232" spans="1:19" s="48" customFormat="1">
       <c r="A232" s="248">
         <v>0.76</v>
       </c>
@@ -62467,7 +62457,7 @@
       <c r="R232" s="58"/>
       <c r="S232" s="58"/>
     </row>
-    <row r="233" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="233" spans="1:19" s="48" customFormat="1">
       <c r="A233" s="248">
         <v>0.76</v>
       </c>
@@ -62504,7 +62494,7 @@
       <c r="R233" s="58"/>
       <c r="S233" s="58"/>
     </row>
-    <row r="234" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="234" spans="1:19" s="48" customFormat="1">
       <c r="A234" s="248">
         <v>0.76</v>
       </c>
@@ -62545,7 +62535,7 @@
       <c r="R234" s="58"/>
       <c r="S234" s="58"/>
     </row>
-    <row r="235" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="235" spans="1:19" s="48" customFormat="1">
       <c r="A235" s="248">
         <v>0.76</v>
       </c>
@@ -62584,7 +62574,7 @@
       <c r="R235" s="58"/>
       <c r="S235" s="58"/>
     </row>
-    <row r="236" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="236" spans="1:19" s="48" customFormat="1">
       <c r="A236" s="248">
         <v>0.76</v>
       </c>
@@ -62635,7 +62625,7 @@
         <v>62600</v>
       </c>
     </row>
-    <row r="237" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="237" spans="1:19" s="48" customFormat="1">
       <c r="A237" s="248">
         <v>0.76</v>
       </c>
@@ -62686,7 +62676,7 @@
         <v>62000</v>
       </c>
     </row>
-    <row r="238" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="238" spans="1:19" s="48" customFormat="1">
       <c r="A238" s="248">
         <v>0.76</v>
       </c>
@@ -62725,7 +62715,7 @@
       <c r="R238" s="58"/>
       <c r="S238" s="58"/>
     </row>
-    <row r="239" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="239" spans="1:19" s="48" customFormat="1">
       <c r="A239" s="248">
         <v>0.76</v>
       </c>
@@ -62776,7 +62766,7 @@
         <v>213847</v>
       </c>
     </row>
-    <row r="240" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="240" spans="1:19" s="48" customFormat="1">
       <c r="A240" s="248">
         <v>0.76</v>
       </c>
@@ -62821,7 +62811,7 @@
       <c r="R240" s="58"/>
       <c r="S240" s="58"/>
     </row>
-    <row r="241" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="241" spans="1:19" s="48" customFormat="1">
       <c r="A241" s="248">
         <v>0.76</v>
       </c>
@@ -62862,7 +62852,7 @@
       <c r="R241" s="58"/>
       <c r="S241" s="58"/>
     </row>
-    <row r="242" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="242" spans="1:19" s="48" customFormat="1">
       <c r="A242" s="248">
         <v>0.76</v>
       </c>
@@ -62909,7 +62899,7 @@
       </c>
       <c r="S242" s="58"/>
     </row>
-    <row r="243" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="243" spans="1:19" s="48" customFormat="1">
       <c r="A243" s="248">
         <v>0.76</v>
       </c>
@@ -62950,7 +62940,7 @@
       <c r="R243" s="58"/>
       <c r="S243" s="58"/>
     </row>
-    <row r="244" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="244" spans="1:19" s="48" customFormat="1">
       <c r="A244" s="248">
         <v>0.76</v>
       </c>
@@ -62991,7 +62981,7 @@
       <c r="R244" s="58"/>
       <c r="S244" s="58"/>
     </row>
-    <row r="245" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="245" spans="1:19" s="48" customFormat="1">
       <c r="A245" s="248">
         <v>0.76</v>
       </c>
@@ -63030,7 +63020,7 @@
       <c r="R245" s="58"/>
       <c r="S245" s="58"/>
     </row>
-    <row r="246" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="246" spans="1:19" s="48" customFormat="1">
       <c r="A246" s="248">
         <v>0.76</v>
       </c>
@@ -63073,7 +63063,7 @@
       </c>
       <c r="S246" s="58"/>
     </row>
-    <row r="247" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="247" spans="1:19" s="48" customFormat="1">
       <c r="A247" s="248">
         <v>0.76</v>
       </c>
@@ -63112,7 +63102,7 @@
       <c r="R247" s="58"/>
       <c r="S247" s="58"/>
     </row>
-    <row r="248" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="248" spans="1:19" s="48" customFormat="1">
       <c r="A248" s="248">
         <v>0.76</v>
       </c>
@@ -63151,7 +63141,7 @@
       <c r="R248" s="58"/>
       <c r="S248" s="58"/>
     </row>
-    <row r="249" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="249" spans="1:19" s="48" customFormat="1">
       <c r="A249" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63206,7 +63196,7 @@
       <c r="R249" s="345"/>
       <c r="S249" s="345"/>
     </row>
-    <row r="250" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="250" spans="1:19" s="48" customFormat="1">
       <c r="A250" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63253,7 +63243,7 @@
       <c r="R250" s="345"/>
       <c r="S250" s="345"/>
     </row>
-    <row r="251" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="251" spans="1:19" s="48" customFormat="1">
       <c r="A251" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63304,7 +63294,7 @@
       <c r="R251" s="345"/>
       <c r="S251" s="345"/>
     </row>
-    <row r="252" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="252" spans="1:19" s="48" customFormat="1">
       <c r="A252" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63353,7 +63343,7 @@
       <c r="R252" s="345"/>
       <c r="S252" s="345"/>
     </row>
-    <row r="253" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="253" spans="1:19" s="48" customFormat="1">
       <c r="A253" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63400,7 +63390,7 @@
       <c r="R253" s="345"/>
       <c r="S253" s="345"/>
     </row>
-    <row r="254" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="254" spans="1:19" s="48" customFormat="1">
       <c r="A254" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63441,7 +63431,7 @@
       <c r="R254" s="345"/>
       <c r="S254" s="345"/>
     </row>
-    <row r="255" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="255" spans="1:19" s="48" customFormat="1">
       <c r="A255" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63484,7 +63474,7 @@
       <c r="R255" s="345"/>
       <c r="S255" s="345"/>
     </row>
-    <row r="256" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="256" spans="1:19" s="48" customFormat="1">
       <c r="A256" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63533,7 +63523,7 @@
       <c r="R256" s="345"/>
       <c r="S256" s="345"/>
     </row>
-    <row r="257" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="257" spans="1:19" s="48" customFormat="1">
       <c r="A257" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63576,7 +63566,7 @@
       <c r="R257" s="345"/>
       <c r="S257" s="345"/>
     </row>
-    <row r="258" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="258" spans="1:19" s="48" customFormat="1">
       <c r="A258" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63617,7 +63607,7 @@
       <c r="R258" s="345"/>
       <c r="S258" s="345"/>
     </row>
-    <row r="259" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="259" spans="1:19" s="48" customFormat="1">
       <c r="A259" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63660,7 +63650,7 @@
       <c r="R259" s="345"/>
       <c r="S259" s="345"/>
     </row>
-    <row r="260" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="260" spans="1:19" s="48" customFormat="1">
       <c r="A260" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63703,7 +63693,7 @@
       <c r="R260" s="345"/>
       <c r="S260" s="345"/>
     </row>
-    <row r="261" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="261" spans="1:19" s="48" customFormat="1">
       <c r="A261" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63744,7 +63734,7 @@
       <c r="R261" s="345"/>
       <c r="S261" s="345"/>
     </row>
-    <row r="262" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="262" spans="1:19" s="48" customFormat="1">
       <c r="A262" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63789,7 +63779,7 @@
       <c r="R262" s="345"/>
       <c r="S262" s="345"/>
     </row>
-    <row r="263" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="263" spans="1:19" s="48" customFormat="1">
       <c r="A263" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63830,7 +63820,7 @@
       <c r="R263" s="345"/>
       <c r="S263" s="345"/>
     </row>
-    <row r="264" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="264" spans="1:19" s="48" customFormat="1">
       <c r="A264" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63881,7 +63871,7 @@
       <c r="R264" s="345"/>
       <c r="S264" s="345"/>
     </row>
-    <row r="265" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="265" spans="1:19" s="48" customFormat="1">
       <c r="A265" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63930,7 +63920,7 @@
       <c r="R265" s="345"/>
       <c r="S265" s="345"/>
     </row>
-    <row r="266" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="266" spans="1:19" s="48" customFormat="1">
       <c r="A266" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -63975,7 +63965,7 @@
       <c r="R266" s="345"/>
       <c r="S266" s="345"/>
     </row>
-    <row r="267" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="267" spans="1:19" s="48" customFormat="1">
       <c r="A267" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64016,7 +64006,7 @@
       <c r="R267" s="345"/>
       <c r="S267" s="345"/>
     </row>
-    <row r="268" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="268" spans="1:19" s="48" customFormat="1">
       <c r="A268" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64057,7 +64047,7 @@
       <c r="R268" s="345"/>
       <c r="S268" s="345"/>
     </row>
-    <row r="269" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="269" spans="1:19" s="48" customFormat="1">
       <c r="A269" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64098,7 +64088,7 @@
       <c r="R269" s="345"/>
       <c r="S269" s="345"/>
     </row>
-    <row r="270" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="270" spans="1:19" s="48" customFormat="1">
       <c r="A270" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64137,7 +64127,7 @@
       <c r="R270" s="345"/>
       <c r="S270" s="345"/>
     </row>
-    <row r="271" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="271" spans="1:19" s="48" customFormat="1">
       <c r="A271" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64182,7 +64172,7 @@
       <c r="R271" s="345"/>
       <c r="S271" s="345"/>
     </row>
-    <row r="272" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="272" spans="1:19" s="48" customFormat="1">
       <c r="A272" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64227,7 +64217,7 @@
       <c r="R272" s="345"/>
       <c r="S272" s="345"/>
     </row>
-    <row r="273" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="273" spans="1:19" s="48" customFormat="1">
       <c r="A273" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64268,7 +64258,7 @@
       <c r="R273" s="345"/>
       <c r="S273" s="345"/>
     </row>
-    <row r="274" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="274" spans="1:19" s="48" customFormat="1">
       <c r="A274" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64307,7 +64297,7 @@
       <c r="R274" s="345"/>
       <c r="S274" s="345"/>
     </row>
-    <row r="275" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="275" spans="1:19" s="48" customFormat="1">
       <c r="A275" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64346,7 +64336,7 @@
       <c r="R275" s="345"/>
       <c r="S275" s="345"/>
     </row>
-    <row r="276" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="276" spans="1:19" s="48" customFormat="1">
       <c r="A276" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -64385,7 +64375,7 @@
       <c r="R276" s="345"/>
       <c r="S276" s="345"/>
     </row>
-    <row r="277" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="277" spans="1:19" s="48" customFormat="1">
       <c r="A277" s="248">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -65324,7 +65314,7 @@
       <c r="R302" s="58"/>
       <c r="S302" s="58"/>
     </row>
-    <row r="303" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="303" spans="1:19" s="48" customFormat="1">
       <c r="A303" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65379,7 +65369,7 @@
       <c r="R303" s="58"/>
       <c r="S303" s="58"/>
     </row>
-    <row r="304" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="304" spans="1:19" s="48" customFormat="1">
       <c r="A304" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65432,7 +65422,7 @@
       <c r="R304" s="58"/>
       <c r="S304" s="58"/>
     </row>
-    <row r="305" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="305" spans="1:19" s="48" customFormat="1">
       <c r="A305" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65487,7 +65477,7 @@
       <c r="R305" s="58"/>
       <c r="S305" s="58"/>
     </row>
-    <row r="306" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="306" spans="1:19" s="48" customFormat="1">
       <c r="A306" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65542,7 +65532,7 @@
       <c r="R306" s="58"/>
       <c r="S306" s="58"/>
     </row>
-    <row r="307" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="307" spans="1:19" s="48" customFormat="1">
       <c r="A307" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65597,7 +65587,7 @@
       <c r="R307" s="58"/>
       <c r="S307" s="58"/>
     </row>
-    <row r="308" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="308" spans="1:19" s="48" customFormat="1">
       <c r="A308" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65650,7 +65640,7 @@
       <c r="R308" s="58"/>
       <c r="S308" s="58"/>
     </row>
-    <row r="309" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="309" spans="1:19" s="48" customFormat="1">
       <c r="A309" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65689,7 +65679,7 @@
       <c r="R309" s="274"/>
       <c r="S309" s="58"/>
     </row>
-    <row r="310" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="310" spans="1:19" s="48" customFormat="1">
       <c r="A310" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65728,7 +65718,7 @@
       <c r="R310" s="274"/>
       <c r="S310" s="58"/>
     </row>
-    <row r="311" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="311" spans="1:19" s="48" customFormat="1">
       <c r="A311" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65767,7 +65757,7 @@
       <c r="R311" s="274"/>
       <c r="S311" s="58"/>
     </row>
-    <row r="312" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="312" spans="1:19" s="48" customFormat="1">
       <c r="A312" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65806,7 +65796,7 @@
       <c r="R312" s="274"/>
       <c r="S312" s="58"/>
     </row>
-    <row r="313" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="313" spans="1:19" s="48" customFormat="1">
       <c r="A313" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65845,7 +65835,7 @@
       <c r="R313" s="274"/>
       <c r="S313" s="58"/>
     </row>
-    <row r="314" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="314" spans="1:19" s="48" customFormat="1">
       <c r="A314" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65884,7 +65874,7 @@
       <c r="R314" s="274"/>
       <c r="S314" s="58"/>
     </row>
-    <row r="315" spans="1:19" s="48" customFormat="1" hidden="1">
+    <row r="315" spans="1:19" s="48" customFormat="1">
       <c r="A315" s="248">
         <v>0.28000000000000003</v>
       </c>
@@ -65926,7 +65916,7 @@
     <row r="316" spans="1:19" ht="13.5" thickBot="1">
       <c r="F316" s="256">
         <f>SUBTOTAL(9,F8:F315)</f>
-        <v>1011652.4450999998</v>
+        <v>68546839.150372252</v>
       </c>
       <c r="G316" s="256"/>
       <c r="H316" s="162"/>
@@ -66498,13 +66488,7 @@
       <c r="E353" s="259"/>
     </row>
   </sheetData>
-  <autoFilter ref="B7:S315" xr:uid="{5389D9F9-F732-4ABD-A2A2-5784FC0C9F5D}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Seychelles"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B7:S315" xr:uid="{5389D9F9-F732-4ABD-A2A2-5784FC0C9F5D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:S248">
     <sortCondition ref="B8:B248"/>
   </sortState>
@@ -66514,7 +66498,7 @@
     <mergeCell ref="C320:E320"/>
   </mergeCells>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>